<commit_message>
Added email sending capability
</commit_message>
<xml_diff>
--- a/logs/log-08-11-2020.xlsx
+++ b/logs/log-08-11-2020.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,19 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>21:54:11</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Penis</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>